<commit_message>
building heap using cpp
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nishc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Personal\DSA\LoveBabbar450Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B5A772-2E5B-4CAF-9FE4-B56CCD4B988E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A339B0-B00A-4E65-853C-69A210E0C6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1872,7 +1872,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="87" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1904,9 +1904,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="C5" s="11" t="s">
-        <v>465</v>
-      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="5" t="s">
@@ -1915,8 +1913,8 @@
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
+      <c r="C6" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -1926,8 +1924,8 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
+      <c r="C7" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">

</xml_diff>